<commit_message>
optimised src of aspect ratio
</commit_message>
<xml_diff>
--- a/usernames_content_data.xlsx
+++ b/usernames_content_data.xlsx
@@ -137,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V4" headerRowCount="1">
-  <autoFilter ref="A1:V4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V7" headerRowCount="1">
+  <autoFilter ref="A1:V7"/>
   <tableColumns count="22">
     <tableColumn id="1" name="Username"/>
     <tableColumn id="2" name="post_type"/>
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>4:5</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -714,7 +714,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>4:5</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -745,10 +745,10 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="U3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V3" t="inlineStr">
         <is>
@@ -792,7 +792,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>16:9</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -829,6 +829,240 @@
         <v>4</v>
       </c>
       <c r="V4" t="inlineStr">
+        <is>
+          <t>Barbil Keonjhar</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>the_year_book_</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DJecytozKis</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-05-10T14:06:03.000Z</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>19</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>07:36 PM</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>4:5</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Do bhai aur Bhagwan ki Kripa se dono tabahi😎🧿💎</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>46</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>700</v>
+      </c>
+      <c r="U5" t="n">
+        <v>33</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Adiyogi Coimbatore</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>the_year_book_</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>DJHpfpGSAcw</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-05-01T17:34:31.000Z</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>23</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>11:04 PM</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>4:5</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Om Namah Shivaya 🙏  #new #shiv #adiyogi</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>40</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>['#new', '#shiv', '#adiyogi']</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>199</v>
+      </c>
+      <c r="U6" t="n">
+        <v>7</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Adiyogi Shiva statue</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>the_year_book_</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DJB1QwfPUKC</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-04-29T11:21:53.000Z</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>16</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>04:51 PM</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>4:5</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Eyes on me!👀 #new #post #blackoutfit</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>37</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['#new', '#post', '#blackoutfit']</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>3</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>114</v>
+      </c>
+      <c r="U7" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" t="inlineStr">
         <is>
           <t>Barbil Keonjhar</t>
         </is>

</xml_diff>

<commit_message>
fixed mark done issue of content level data
</commit_message>
<xml_diff>
--- a/usernames_content_data.xlsx
+++ b/usernames_content_data.xlsx
@@ -137,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V7" headerRowCount="1">
-  <autoFilter ref="A1:V7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V6" headerRowCount="1">
+  <autoFilter ref="A1:V6"/>
   <tableColumns count="22">
     <tableColumn id="1" name="Username"/>
     <tableColumn id="2" name="post_type"/>
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="U5" t="n">
         <v>33</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U6" t="n">
         <v>7</v>
@@ -987,84 +987,6 @@
       <c r="V6" t="inlineStr">
         <is>
           <t>Adiyogi Shiva statue</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>the_year_book_</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Post</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>DJB1QwfPUKC</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-04-29T11:21:53.000Z</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Tuesday</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>16</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>04:51 PM</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>4:5</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Eyes on me!👀 #new #post #blackoutfit</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>37</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>['#new', '#post', '#blackoutfit']</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>3</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
-        <v>114</v>
-      </c>
-      <c r="U7" t="n">
-        <v>1</v>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Barbil Keonjhar</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
optimised content level data and profile level data saving
</commit_message>
<xml_diff>
--- a/usernames_content_data.xlsx
+++ b/usernames_content_data.xlsx
@@ -667,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="U2" t="n">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="U3" t="n">
         <v>3</v>
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>702</v>
+        <v>720</v>
       </c>
       <c r="U5" t="n">
         <v>33</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="U6" t="n">
         <v>7</v>

</xml_diff>

<commit_message>
optimised next post to be fetched
</commit_message>
<xml_diff>
--- a/usernames_content_data.xlsx
+++ b/usernames_content_data.xlsx
@@ -137,8 +137,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V11" headerRowCount="1">
-  <autoFilter ref="A1:V11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="contentDataTable" displayName="contentDataTable" ref="A1:V42" headerRowCount="1">
+  <autoFilter ref="A1:V42"/>
   <tableColumns count="22">
     <tableColumn id="1" name="Username"/>
     <tableColumn id="2" name="post_type"/>
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,7 +603,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>just.sujal.yk</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -613,30 +613,30 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DHjHudCTzxI</t>
+          <t>DCEvmGcydui</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-23T16:36:07.000Z</t>
+          <t>2024-11-07T14:57:42.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>10:06 PM</t>
+          <t>08:27 PM</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>01:11</t>
+          <t>00:17</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -646,22 +646,22 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>HYPER HAI!!! (RAP) #rap</t>
+          <t>Hasad ( Jalan ) Karna nahi Chahiye. Dene wali Zaat Sirf Allahﷻ ki hai .🤲✨️</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>['#rap']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -677,16 +677,16 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>65</v>
+        <v>36419</v>
       </c>
       <c r="U2" t="n">
-        <v>46</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>just.sujal.yk</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -696,72 +696,80 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DGgFqt7zG4J</t>
+          <t>DCCJWVAyqih</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-02-25T15:48:17.000Z</t>
+          <t>2024-11-06T14:44:03.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>09:18 PM</t>
+          <t>08:14 PM</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>00:04</t>
+          <t>00:42</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4:5</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Kavi kehna chahte hein ki.</t>
+          <t>Only feel And Share... ✨️  . . . . .  Original voice is from @miah_kutty_official Such a heart touching voice #feel  #reelitfeelit  #sound  #cutevoice  #voice  #explorepage</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#feel', '#reelitfeelit', '#sound', '#cutevoice', '#voice', '#explorepage']</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['@miah_kutty_official']</t>
         </is>
       </c>
       <c r="P3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
       </c>
       <c r="T3" t="n">
-        <v>59</v>
+        <v>7014406</v>
+      </c>
+      <c r="U3" t="n">
+        <v>70712</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>just.sujal.yk</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -771,30 +779,30 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DD6oN7FTG-m</t>
+          <t>DJ_9TktT_pQ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-12-23T09:37:28.000Z</t>
+          <t>2025-05-23T14:26:39.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>03:07 PM</t>
+          <t>07:56 PM</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>01:36</t>
+          <t>00:13</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -804,22 +812,22 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>RAP SONG FOR THE REAL ONES.  Dost hain - Sujal Karmakar</t>
+          <t>Very Chalak billa 😸  #cat #catlovers #viralreels #funnyreels #reels</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="L4" t="n">
         <v>2</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#cat', '#catlovers', '#viralreels', '#funnyreels', '#reels']</t>
         </is>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -831,73 +839,78 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>original</t>
+          <t>Shankar Mahadevan, Siddharth Mahadevan, Divya Kumar, Shankar Ehsaan LoySitaare Zameen Par Teaser</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>82</v>
+        <v>1672</v>
       </c>
       <c r="U4" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>just.sujal.yk</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Reel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CjTeDsqhyh4</t>
+          <t>DJ9SGydTYYr</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-10-04T19:52:29.000Z</t>
+          <t>2025-05-22T13:29:45.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>01:22 AM</t>
+          <t>06:59 PM</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>00:08</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>E equals MC squared I've got a blimp inside my head.. . . . . . Navami. end of festivities.</t>
+          <t>#nofilterchallenge #amaira #challenge #ReelKaroFeelKaro #fypシ゚</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="L5" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#nofilterchallenge', '#amaira', '#challenge', '#ReelKaroFeelKaro', '#fypシ']</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -907,70 +920,80 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
       <c r="T5" t="n">
-        <v>121</v>
+        <v>3143</v>
       </c>
       <c r="U5" t="n">
-        <v>21</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>just.sujal.yk</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Reel</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CgtiJwHBsQj</t>
+          <t>DJ6mEozzFYB</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-08-01T09:14:20.000Z</t>
+          <t>2025-05-21T12:34:16.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>02:44 PM</t>
+          <t>06:04 PM</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>00:50</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>4:5</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>DOPEST IN THE ROOM.</t>
+          <t>Mere Matlab ka Jawab nahi diya inhone 😝🤣  #funnyreels #cute #ReelKaroFeelKaro  #funny #amaira #trending</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#funnyreels', '#cute', '#ReelKaroFeelKaro', '#funny', '#amaira', '#trending']</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -980,139 +1003,159 @@
       <c r="P6" t="n">
         <v>0</v>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Amaira ki Baat</t>
+        </is>
+      </c>
       <c r="T6" t="n">
-        <v>88</v>
+        <v>4343</v>
       </c>
       <c r="U6" t="n">
-        <v>33</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ashishchanchlani</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Reel</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DJD7-M0IIak</t>
+          <t>DJzGkYQTlqW</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-04-30T06:59:00.000Z</t>
+          <t>2025-05-18T14:37:58.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>12:29 PM</t>
+          <t>08:07 PM</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>00:17</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>4:5</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>We whole heartedly invite you for the chilliest trip of the year  Bas yaad rakhna..  EKAKI mein reh kar bhi aap kabhi akele nahi rahenge🧟‍♂️  Co passengers : @akashdodeja @harshhrane @sidhantsarfare @mrrohitsadhwani @shashankshekhrr @grishim_nawanii @akshayalokk  Coming soon exclusively on YOUTUBE.  #Ekaki #ashishchanchlani #AcvStudios</t>
+          <t>Little💗 Baby 💕 @a4amaira   #cutebaby #cuteamaira  #cute #littlebaby #californiagirl  #fyp #girl #prettygirls</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>348</v>
+        <v>112</v>
       </c>
       <c r="L7" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>['#Ekaki', '#ashishchanchlani', '#AcvStudios']</t>
+          <t>['#cutebaby', '#cuteamaira', '#cute', '#littlebaby', '#californiagirl', '#fyp', '#girl', '#prettygirls']</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>['@akashdodeja', '@harshhrane', '@sidhantsarfare', '@mrrohitsadhwani', '@shashankshekhrr', '@grishim_nawanii', '@akshayalokk']</t>
+          <t>['@a4amaira']</t>
         </is>
       </c>
       <c r="P7" t="n">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Connie Francis•Pretty Little Baby</t>
+        </is>
       </c>
       <c r="T7" t="n">
-        <v>1344558</v>
+        <v>2351</v>
       </c>
       <c r="U7" t="n">
-        <v>14272</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ashishchanchlani</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Reel</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>DDTniMRoD8N</t>
+          <t>DJwebUOzn5h</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-12-08T05:59:54.000Z</t>
+          <t>2025-05-17T14:09:21.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>11:29 AM</t>
+          <t>07:39 PM</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>00:13</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4:5</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Comedy of errors or comedy of horrors 👹 You decide #Acv159  can you guess the star cast?  Coincidently, Today on my birthday i complete 10 years in the youtube industry. And as my new phase begins  as a creator as well as ashu myself, i am proud to tell you all we are launching our own production house @AcvStudios_ With this new beginning we are elated to tell you exciting fresh stories from our heartland filled not just with comedy, but horror, thrills and yes emotions as well This project is my love letter to every ACVIAN  Thank you for being there See you on YOUTUBE 👀😈 #Acv159 #AcvStudios #AshishChanchlani</t>
+          <t>Mobile me bhi nahi samai 😁 @awesome.aysha Mumma 😁😁😁  #reelkrofeelkro #reel #funnyreels #explore</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>624</v>
+        <v>97</v>
       </c>
       <c r="L8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>['#Acv159', '#Acv159', '#AcvStudios', '#AshishChanchlani']</t>
+          <t>['#reelkrofeelkro', '#reel', '#funnyreels', '#explore']</t>
         </is>
       </c>
       <c r="N8" t="n">
@@ -1120,23 +1163,28 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>['@AcvStudios_']</t>
+          <t>['@awesome']</t>
         </is>
       </c>
       <c r="P8" t="n">
         <v>1</v>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>funn AMAIRA</t>
+        </is>
+      </c>
       <c r="T8" t="n">
-        <v>453800</v>
+        <v>4421</v>
       </c>
       <c r="U8" t="n">
-        <v>3442</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ashishchanchlani</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1146,30 +1194,30 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DABFeaCo2WU</t>
+          <t>DJt-ZBqz1l7</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-09-17T11:44:06.000Z</t>
+          <t>2025-05-16T14:53:48.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>05:14 PM</t>
+          <t>08:23 PM</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>00:46</t>
+          <t>00:10</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1179,47 +1227,47 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>a story you will never believe… See you on the other side 😈  #ACV159</t>
+          <t>Lo bana diya Thank you #instafamily itna #support karne k liye ..🫡😁😍 Jenny @a4amaira Khush hui.....  #movies #reels  #jenny #explore  #repost #instagram  #movies #cutevoice</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="L9" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>['#ACV159']</t>
+          <t>['#instafamily', '#support', '#movies', '#reels', '#jenny', '#explore', '#repost', '#instagram', '#movies', '#cutevoice']</t>
         </is>
       </c>
       <c r="N9" t="n">
+        <v>10</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>['@a4amaira']</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
         <v>1</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
       <c r="Q9" t="inlineStr">
         <is>
           <t>original</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>858585</v>
+        <v>6737</v>
       </c>
       <c r="U9" t="n">
-        <v>7494</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ashishchanchlani</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1229,30 +1277,30 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DJeJqIso4Ie</t>
+          <t>DJrRNCizSBK</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-05-10T11:21:23.000Z</t>
+          <t>2025-05-15T13:35:44.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>04:51 PM</t>
+          <t>07:05 PM</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>01:36</t>
+          <t>00:10</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1262,22 +1310,22 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Not one single message of peace was sent during pulawama, 26/11 or even the recent pahalgam attack. Whats the new definition of peace? Playing victim card after poking for years? Know the truth before blindly defending🙏 जय हिन्द🇮🇳</t>
+          <t>Farak nahi padta 😄  #marriage #shadi #cutebaby #cute  #amaira #explore  #ReelKaroFeelKaro</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>233</v>
+        <v>93</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#marriage', '#shadi', '#cutebaby', '#cute', '#amaira', '#explore', '#ReelKaroFeelKaro']</t>
         </is>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1293,69 +1341,74 @@
         </is>
       </c>
       <c r="T10" t="n">
-        <v>749844</v>
+        <v>4471</v>
       </c>
       <c r="U10" t="n">
-        <v>28211</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ashishchanchlani</t>
+          <t>a4amaira</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Post</t>
+          <t>Reel</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>DHdFIjSIjqk</t>
+          <t>DJmEl-1zz6f</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-03-21T08:17:17.000Z</t>
+          <t>2025-05-13T13:09:36.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>01:47 PM</t>
+          <t>06:39 PM</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>00:09</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4:5</t>
+          <t>9:16</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Kaafi stress eating ho gayi bhai🤣 batao ab kab aaye wapis👀</t>
+          <t>Jenny Dar Gaai 😄  #movies #reel</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['#movies', '#reel']</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1365,11 +1418,2584 @@
       <c r="P11" t="n">
         <v>0</v>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
       <c r="T11" t="n">
-        <v>957526</v>
+        <v>186663</v>
       </c>
       <c r="U11" t="n">
-        <v>3654</v>
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>DJje67LTsFx</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-05-12T13:04:06.000Z</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>18</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>06:34 PM</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>00:07</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Aap sunao 😁  #alphabet #cuteammie #explore #funnyreels #explore  #reels #cute #cutevoice</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>91</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['#alphabet', '#cuteammie', '#explore', '#funnyreels', '#explore', '#reels', '#cute', '#cutevoice']</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>8</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>cuteamaira</t>
+        </is>
+      </c>
+      <c r="T12" t="n">
+        <v>5900</v>
+      </c>
+      <c r="U12" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>DJfoKKJTGFS</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-05-11T01:12:35.000Z</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>06:42 AM</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>00:44</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Maa ne sikhaya chalna, bolna,🥰 Maa ne sikhaya sapne dekhna. 😘 Kabhi dantti hai, kabhi pyar karti hai,🫡 Par kabhi pyaar kam nahi karti! ❤️  @awesome.aysha</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>157</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Kailash Kher•Mumma</t>
+        </is>
+      </c>
+      <c r="T13" t="n">
+        <v>3726</v>
+      </c>
+      <c r="U13" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DJeKE-4T9_b</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-05-10T11:26:37.000Z</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>16</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>04:56 PM</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>00:58</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Happy Mother's day 🌺 mumma @awesome.aysha</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>42</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Atif Aslam, Pritam Chakraborty•Janam Janam (Sad Version)</t>
+        </is>
+      </c>
+      <c r="T14" t="n">
+        <v>16824</v>
+      </c>
+      <c r="U14" t="n">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>DJZQw1mTcaE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-05-08T13:48:36.000Z</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>19</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>07:18 PM</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>00:25</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Apni Suno bhaiyya 🤫🤔😆.....  #reels #Explore #feature #cuteammie</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>65</v>
+      </c>
+      <c r="L15" t="n">
+        <v>2</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>['#reels', '#Explore', '#feature', '#cuteammie']</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>4</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T15" t="n">
+        <v>4738</v>
+      </c>
+      <c r="U15" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>DJWq__pzB54</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-05-07T13:38:09.000Z</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>19</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>07:08 PM</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Wo 😳🤐 @awesome.aysha kya..?  #reels #realstories</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>50</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>['#reels', '#realstories']</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>2</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Yo Yo Honey Singh, Simar Kaur, Alfaaz•Laal Pari (From "Housefull 5")</t>
+        </is>
+      </c>
+      <c r="T16" t="n">
+        <v>19280</v>
+      </c>
+      <c r="U16" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>DJUEpWXzX5w</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-05-06T13:24:29.000Z</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>18</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>06:54 PM</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>00:31</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Chehre ki Chamak 🤐 ......  #reels</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>35</v>
+      </c>
+      <c r="L17" t="n">
+        <v>2</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>['#reels']</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>1</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Future, Metro Boomin, Travis Scott, Playboi Carti•Type Shit</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>2161</v>
+      </c>
+      <c r="U17" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>DJRpxUlzQF-</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-05-05T14:50:06.000Z</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>20</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>08:20 PM</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>00:10</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Hahaa @awesome.aysha samajh gaai Pyari amma 🤣🤣🤣  #reels</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>57</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>['#reels']</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>1</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>filter</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>3705</v>
+      </c>
+      <c r="U18" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>DJMtYzqzw5O</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-05-03T16:47:34.000Z</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>22</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10:17 PM</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>00:36</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Tharki bhai @a4ashaaz 😂😳😭😭🤣🤣  #tharki #tharkiladka #funny  #funnyvideos #viralreels #explore</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>95</v>
+      </c>
+      <c r="L19" t="n">
+        <v>3</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>['#tharki', '#tharkiladka', '#funny', '#funnyvideos', '#viralreels', '#explore']</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>6</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>['@a4ashaaz']</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Jawad Ahmed, Sharib Toshi, Shreya Ghoshal, Arijit Singh•Tenu Chad Ke (Samjhawan - Trending Version)</t>
+        </is>
+      </c>
+      <c r="T19" t="n">
+        <v>2435</v>
+      </c>
+      <c r="U19" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>DJJ_eTkzGyM</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-05-02T15:28:11.000Z</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>08:58 PM</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>00:17</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>♥️ only Feel this #voice ........  #voices #song #music #cute  #reels #fypシ゚</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>79</v>
+      </c>
+      <c r="L20" t="n">
+        <v>3</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>['#voice', '#voices', '#song', '#music', '#cute', '#reels', '#fypシ']</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>7</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>cutevoice</t>
+        </is>
+      </c>
+      <c r="T20" t="n">
+        <v>3719</v>
+      </c>
+      <c r="U20" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>DJHVECQThpU</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-05-01T14:35:46.000Z</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>20</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>08:05 PM</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>00:19</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Aysa Password 😒🤔😳😢.....  Password #explore  #reels #funny</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>60</v>
+      </c>
+      <c r="L21" t="n">
+        <v>3</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>['#explore', '#reels', '#funny']</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>3</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Kailash Kher•Mumma</t>
+        </is>
+      </c>
+      <c r="T21" t="n">
+        <v>2116</v>
+      </c>
+      <c r="U21" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>DJCGtxHTCXU</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-04-29T13:56:27.000Z</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>19</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>07:26 PM</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>00:22</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Humdardi padi Bhari 😳 wo bhi @awesome.aysha ammi k sath 😭 Lakin bhaut maza aaya... 😂🤣 . . . . #humdard #explore #reels #reelkrofeelkro #reelsinstagram #trending #cuteammie #funny</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>184</v>
+      </c>
+      <c r="L22" t="n">
+        <v>6</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>['#humdard', '#explore', '#reels', '#reelkrofeelkro', '#reelsinstagram', '#trending', '#cuteammie', '#funny']</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>8</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Mithoon, Arijit Singh•Humdard</t>
+        </is>
+      </c>
+      <c r="T22" t="n">
+        <v>2308</v>
+      </c>
+      <c r="U22" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>DI_kdkcTNNi</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-04-28T14:20:25.000Z</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>19</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>07:50 PM</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>00:44</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Aap log Zyada se Zyada Dua Kariye or video ko zyada share kariye jisse @syeed_bilal_abid Bhai ko zyada mil madad sake ... Allah inki Ye Bimari Door kare Ameen....   #support</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>176</v>
+      </c>
+      <c r="L23" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>['#support']</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>1</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>['@syeed_bilal_abid']</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Al Haaj Muhammad Owais Raza Qadri•Karam Mangta Hun</t>
+        </is>
+      </c>
+      <c r="T23" t="n">
+        <v>62017</v>
+      </c>
+      <c r="U23" t="n">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>DI8Uc3bz1FG</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-04-27T08:06:17.000Z</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>13</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>01:36 PM</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>00:10</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Kis kis k yaha ye Problem hai Comment box open hai batane ko ...😆  #fridge #viralreels #reels #trendingreels #cuteammie #reelkrofeelkro</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>140</v>
+      </c>
+      <c r="L24" t="n">
+        <v>5</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>['#fridge', '#viralreels', '#reels', '#trendingreels', '#cuteammie', '#reelkrofeelkro']</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>6</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T24" t="n">
+        <v>3677</v>
+      </c>
+      <c r="U24" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>DI3DlFjTNcx</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-04-25T06:58:41.000Z</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>12</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>12:28 PM</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>00:18</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Har Musibat ko Talti hai dua🤲🤲✨️✨️.......  #dua #islamkishehzadi #islamicgirl #explore   #reelkrofeelkro #reels</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>115</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>['#dua', '#islamkishehzadi', '#islamicgirl', '#explore', '#reelkrofeelkro', '#reels']</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>6</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T25" t="n">
+        <v>5402</v>
+      </c>
+      <c r="U25" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>DIy0TCETWqA</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2025-04-23T15:31:13.000Z</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>21</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>09:01 PM</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>00:28</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Tag - 💃🐒 .... 🤣🤣🤣  #funnyreels #tags #viralreels #reels</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>57</v>
+      </c>
+      <c r="L26" t="n">
+        <v>2</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>['#funnyreels', '#tags', '#viralreels', '#reels']</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>4</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>gladdestofficiall•Gladdest-Done with your ex</t>
+        </is>
+      </c>
+      <c r="T26" t="n">
+        <v>2300</v>
+      </c>
+      <c r="U26" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>DIyitugTmo9</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2025-04-23T12:53:01.000Z</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>18</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>06:23 PM</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>00:13</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Kuchh manga raha hu mai..  #cutevoice #cute #baby #reels</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>57</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>['#cutevoice', '#cute', '#baby', '#reels']</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>4</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T27" t="n">
+        <v>2259</v>
+      </c>
+      <c r="U27" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DIqPLDSTFxC</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2025-04-20T07:26:57.000Z</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>12</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>12:56 PM</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>00:10</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>🤣🤣 #doors #funnyreels #reels #reelkrofeelkro</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>44</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>['#doors', '#funnyreels', '#reels', '#reelkrofeelkro']</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>4</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Devx Sidhu•Secrets</t>
+        </is>
+      </c>
+      <c r="T28" t="n">
+        <v>3143</v>
+      </c>
+      <c r="U28" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Post</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>DIk3lLyToMe</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2025-04-18T05:24:11.000Z</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>10</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>10:54 AM</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>4:5</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Allah’s mercy ♥️ is greater than your sins. 🕋 ALLAH Says in Quran 14:7 "If you are grateful, I will surely increase you." 🤲✨️✨️  #mercy #allah #allahﷻ #islamicpage #islam #islamicstatus  #islamkishehzadi  #ᴀʟʟᴀʜᴜᴀᴋʙᴀʀ  #postoftheday  #jummahmubarak</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>260</v>
+      </c>
+      <c r="L29" t="n">
+        <v>12</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>['#mercy', '#allah', '#allahﷻ', '#islamicpage', '#islam', '#islamicstatus', '#islamkishehzadi', '#ᴀʟʟᴀʜᴜᴀᴋʙᴀʀ', '#postoftheday', '#jummahmubarak']</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>10</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>4014</v>
+      </c>
+      <c r="U29" t="n">
+        <v>90</v>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>Jummah Mubarak</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>DIjRgLnzsN7</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2025-04-17T14:32:54.000Z</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>20</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>08:02 PM</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>00:10</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Mera hi Dil ♥️ 🥰 #cute #cutebaby #explore #viralreels #reels</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>60</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>['#cute', '#cutebaby', '#explore', '#viralreels', '#reels']</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>5</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>5361</v>
+      </c>
+      <c r="U30" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>DIgqbv9SD7I</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2025-04-16T14:16:48.000Z</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>19</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>07:46 PM</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>00:19</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Papa ki Pari 🧚‍♂️ 👸 😂😂  #papakipari #cuteamaira #reels #reelkrofeelkro</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>72</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>['#papakipari', '#cuteamaira', '#reels', '#reelkrofeelkro']</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>4</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>papa ki pari</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>3599</v>
+      </c>
+      <c r="U31" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>DIeOkAJTaVL</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2025-04-15T15:30:01.000Z</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>21</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>09:00 PM</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>00:15</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Aay Bhai💡 ye Q Chali gaai Garmi bahut hai...😱 I</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>48</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T32" t="n">
+        <v>2463</v>
+      </c>
+      <c r="U32" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>DIZFXBJTU1N</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2025-04-13T15:42:43.000Z</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>21</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>09:12 PM</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>00:16</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Ye kaise Reel Bana di 😱Bhai Mumma to Kahi bhi Beizzati kara deti hai 😡🥺😭    #reels #reelkrofeelkro</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>101</v>
+      </c>
+      <c r="L33" t="n">
+        <v>3</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>['#reels', '#reelkrofeelkro']</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>2</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T33" t="n">
+        <v>2314</v>
+      </c>
+      <c r="U33" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>DIRLMm5z_LN</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2025-04-10T13:51:06.000Z</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>19</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>07:21 PM</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>00:09</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Bhai meri khushi ☺️😄  #explore #ReelKaroFeelKaro  #reels</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>59</v>
+      </c>
+      <c r="L34" t="n">
+        <v>3</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>['#explore', '#ReelKaroFeelKaro', '#reels']</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>3</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T34" t="n">
+        <v>4195</v>
+      </c>
+      <c r="U34" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>DIOva9zTdIP</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2025-04-09T15:10:27.000Z</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>20</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>08:40 PM</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>00:20</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Mujhe to Instagram Mila 😱  @awesome.aysha   #instagram #instafamily #insta #reels #explore</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>93</v>
+      </c>
+      <c r="L35" t="n">
+        <v>3</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>['#instagram', '#instafamily', '#insta', '#reels', '#explore']</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>5</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T35" t="n">
+        <v>5321</v>
+      </c>
+      <c r="U35" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>DIMDBZhsBNN</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2025-04-08T14:04:29.000Z</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>19</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>07:34 PM</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>00:09</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Bahut Bada dukh hai 🥺 @a4amaira   #viralreels #explore #reels</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>63</v>
+      </c>
+      <c r="L36" t="n">
+        <v>2</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>['#viralreels', '#explore', '#reels']</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>3</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>['@a4amaira']</t>
+        </is>
+      </c>
+      <c r="P36" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T36" t="n">
+        <v>61896</v>
+      </c>
+      <c r="U36" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>DIJh31OMpvl</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2025-04-07T14:53:05.000Z</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>20</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>08:23 PM</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>00:27</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Aysay kon Puchhta hai bhai. 🫠🥸😡😋 Biryani thi yaar 😒 😑 😢   #biryani #reels</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>75</v>
+      </c>
+      <c r="L37" t="n">
+        <v>2</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>['#biryani', '#reels']</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>2</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>Arijit Singh•Aa Seetadevi Navvula</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>4662</v>
+      </c>
+      <c r="U37" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>DIGwlIjMJSf</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2025-04-06T12:46:48.000Z</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>18</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>06:16 PM</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>00:07</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Tag Your Kalua Chala 🤣  #kalua #explore #reels #reelkrofeelkro #explore</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>73</v>
+      </c>
+      <c r="L38" t="n">
+        <v>2</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>['#kalua', '#explore', '#reels', '#reelkrofeelkro', '#explore']</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>5</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>3132</v>
+      </c>
+      <c r="U38" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>DIEUCMbTsuM</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2025-04-05T13:58:37.000Z</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>19</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>07:28 PM</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>00:10</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Khatam ..💸🫢  #eid #viralreels #explore #reelsinstagram #explore</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>65</v>
+      </c>
+      <c r="L39" t="n">
+        <v>2</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>['#eid', '#viralreels', '#explore', '#reelsinstagram', '#explore']</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>5</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T39" t="n">
+        <v>3581</v>
+      </c>
+      <c r="U39" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>DIBnjxQzaEJ</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2025-04-04T12:50:43.000Z</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>18</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>06:20 PM</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>00:28</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Dar ka Mahol ☠️💸😱🫢 @shahnawaz.sidd84  #cuteamaira #viralreels #explore #trendingreels #reels #reelkrofeelkro</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>110</v>
+      </c>
+      <c r="L40" t="n">
+        <v>2</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>['#cuteamaira', '#viralreels', '#explore', '#trendingreels', '#reels', '#reelkrofeelkro']</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>6</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>['@shahnawaz']</t>
+        </is>
+      </c>
+      <c r="P40" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>Suman Sridhar•Muskaanein Jhooti Hai</t>
+        </is>
+      </c>
+      <c r="T40" t="n">
+        <v>11205</v>
+      </c>
+      <c r="U40" t="n">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>DH8quSSTOnz</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2025-04-02T14:42:29.000Z</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Wednesday</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>20</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>08:12 PM</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>00:08</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Deal Pakki hui 💸😄 @awesome.aysha  #money #mom #eidi #explore</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>62</v>
+      </c>
+      <c r="L41" t="n">
+        <v>2</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>['#money', '#mom', '#eidi', '#explore']</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>4</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>['@awesome']</t>
+        </is>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+      <c r="T41" t="n">
+        <v>3397</v>
+      </c>
+      <c r="U41" t="n">
+        <v>48</v>
+      </c>
+      <c r="V41" t="inlineStr">
+        <is>
+          <t>Mumbai - The City of Dreams</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>a4amaira</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Reel</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>DH4_EIDTQ4z</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2025-04-01T04:24:49.000Z</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>9</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>09:54 AM</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>00:14</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>9:16</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Eidi Na De Wo Kanjoos 🙄 jaldi eidi dedo....  #eidi #eid #explore #fypシ゚</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>73</v>
+      </c>
+      <c r="L42" t="n">
+        <v>2</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>['#eidi', '#eid', '#explore', '#fypシ']</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>4</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>original</t>
+        </is>
+      </c>
+      <c r="T42" t="n">
+        <v>11585</v>
+      </c>
+      <c r="U42" t="n">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>